<commit_message>
Player data output and cleanup
</commit_message>
<xml_diff>
--- a/data/game_data/npc_station_ids.xlsx
+++ b/data/game_data/npc_station_ids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana\Documents\Python Projects\Eve Production Auto\data\game_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A4359-26D4-4B92-B3C8-8753B978E297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143D394C-1562-4A92-9028-DB8E7D99139D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3670" yWindow="3150" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5133" uniqueCount="5133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5134" uniqueCount="5134">
   <si>
     <t>0G-A25 VI - Moon 20 - True Power Mining Outpost</t>
   </si>
@@ -15424,6 +15424,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Hek IX - Paragon Fulfillment Center</t>
   </si>
 </sst>
 </file>
@@ -15744,10 +15747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5132"/>
+  <dimension ref="A1:B5133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A5126" workbookViewId="0">
+      <selection activeCell="F5127" sqref="F5127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56808,7 +56811,16 @@
         <v>5130</v>
       </c>
     </row>
+    <row r="5133" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5133" s="1">
+        <v>60015171</v>
+      </c>
+      <c r="B5133" s="1" t="s">
+        <v>5133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>